<commit_message>
Extraction now writes time elapsed
</commit_message>
<xml_diff>
--- a/extraction_summary.xlsx
+++ b/extraction_summary.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
@@ -1616,6 +1616,50 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1741</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1851</v>
+      </c>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1633</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>33.28</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>35.38</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>31.21</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>2025-09-01 20:29:32</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>